<commit_message>
removed xdo metadata sheet
</commit_message>
<xml_diff>
--- a/01-data/ofsll_open_interface_manual_servicing.xlsx
+++ b/01-data/ofsll_open_interface_manual_servicing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tpathan\Downloads\train\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD15B5B-932D-4827-931A-4172F5D90931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF15CE5-7607-4E9A-8358-43A633E5A832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="29" activeTab="32" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="API_CONTRACTS" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,6 @@
     <sheet name="API_CUSTOMER_CREDIT_SCORE" sheetId="32" r:id="rId31"/>
     <sheet name="API_BUSINESS_CREDIT_SCORE" sheetId="33" r:id="rId32"/>
     <sheet name="API_TRADE_DETAILS" sheetId="34" r:id="rId33"/>
-    <sheet name="XDO_METADATA" sheetId="35" r:id="rId34"/>
   </sheets>
   <definedNames>
     <definedName name="XDO_?XDOFIELD1?">API_CONTRACTS!$A$3:$A$158</definedName>
@@ -385,7 +384,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14511" uniqueCount="2823">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14479" uniqueCount="2791">
   <si>
     <t>OFSLL Field Mapping for Conversion</t>
   </si>
@@ -8758,102 +8757,6 @@
   </si>
   <si>
     <t>Current indicator</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>ARU-dbdrv</t>
-  </si>
-  <si>
-    <t>Extractor Version</t>
-  </si>
-  <si>
-    <t>Template Code</t>
-  </si>
-  <si>
-    <t>Template Type</t>
-  </si>
-  <si>
-    <t>TYPE_EXCEL_TEMPLATE</t>
-  </si>
-  <si>
-    <t>Preprocess XSLT File</t>
-  </si>
-  <si>
-    <t>Last Modified Date</t>
-  </si>
-  <si>
-    <t>Last Modified By</t>
-  </si>
-  <si>
-    <t>Data Constraints:</t>
-  </si>
-  <si>
-    <t>XDO_?XDOFIELD1?</t>
-  </si>
-  <si>
-    <t>&lt;?COL_NAME?&gt;</t>
-  </si>
-  <si>
-    <t>XDO_?XDOFIELD2?</t>
-  </si>
-  <si>
-    <t>&lt;?COL_TYPE?&gt;</t>
-  </si>
-  <si>
-    <t>XDO_?XDOFIELD3?</t>
-  </si>
-  <si>
-    <t>&lt;?COL_LENGTH?&gt;</t>
-  </si>
-  <si>
-    <t>XDO_?XDOFIELD4?</t>
-  </si>
-  <si>
-    <t>&lt;?COL_NULLABLE?&gt;</t>
-  </si>
-  <si>
-    <t>XDO_?XDOFIELD5?</t>
-  </si>
-  <si>
-    <t>&lt;?COL_COMMENTS?&gt;</t>
-  </si>
-  <si>
-    <t>XDO_?XDOFIELD6?</t>
-  </si>
-  <si>
-    <t>&lt;?COL_LOOKUP?&gt;</t>
-  </si>
-  <si>
-    <t>XDO_?XDOFIELD7?</t>
-  </si>
-  <si>
-    <t>&lt;?COL_LN_REQ?&gt;</t>
-  </si>
-  <si>
-    <t>XDO_?XDOFIELD8?</t>
-  </si>
-  <si>
-    <t>&lt;?COL_LS_REQ?&gt;</t>
-  </si>
-  <si>
-    <t>XDO_?XDOFIELD9?</t>
-  </si>
-  <si>
-    <t>&lt;?COL_LOC_REQ?&gt;</t>
-  </si>
-  <si>
-    <t>XDO_SHEET_?</t>
-  </si>
-  <si>
-    <t>&lt;?.//G_TABNAME?&gt;</t>
-  </si>
-  <si>
-    <t>XDO_SHEET_NAME_?</t>
-  </si>
-  <si>
-    <t>&lt;?.//TAB_NAME?&gt;</t>
   </si>
 </sst>
 </file>
@@ -9294,7 +9197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -44699,8 +44602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45069,161 +44972,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
-  <dimension ref="A1:B21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2791</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2792</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2793</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2794</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2795</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2796</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>2797</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>2798</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>2799</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>2800</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>2801</v>
-      </c>
-      <c r="B11" t="s">
-        <v>2802</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>2803</v>
-      </c>
-      <c r="B12" t="s">
-        <v>2804</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>2805</v>
-      </c>
-      <c r="B13" t="s">
-        <v>2806</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>2807</v>
-      </c>
-      <c r="B14" t="s">
-        <v>2808</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>2809</v>
-      </c>
-      <c r="B15" t="s">
-        <v>2810</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>2811</v>
-      </c>
-      <c r="B16" t="s">
-        <v>2812</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>2813</v>
-      </c>
-      <c r="B17" t="s">
-        <v>2814</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>2815</v>
-      </c>
-      <c r="B18" t="s">
-        <v>2816</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>2817</v>
-      </c>
-      <c r="B19" t="s">
-        <v>2818</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>2819</v>
-      </c>
-      <c r="B20" t="s">
-        <v>2820</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>2821</v>
-      </c>
-      <c r="B21" t="s">
-        <v>2822</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>